<commit_message>
fixed up the tranistions to match the diagram
</commit_message>
<xml_diff>
--- a/Project 1 milestone/State Tranistions_project1.xlsx
+++ b/Project 1 milestone/State Tranistions_project1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Documents\GitHub\CMPT440\Project 1 milestone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\colin\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21525" windowHeight="13275"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="111">
   <si>
     <t>Q0</t>
   </si>
@@ -233,9 +233,6 @@
     <t>q40</t>
   </si>
   <si>
-    <t>q2,q28</t>
-  </si>
-  <si>
     <t>q3</t>
   </si>
   <si>
@@ -263,9 +260,6 @@
     <t>q11</t>
   </si>
   <si>
-    <t>q12</t>
-  </si>
-  <si>
     <t>q13</t>
   </si>
   <si>
@@ -290,18 +284,9 @@
     <t>q20</t>
   </si>
   <si>
-    <t>q23</t>
-  </si>
-  <si>
-    <t>q28</t>
-  </si>
-  <si>
     <t>q48</t>
   </si>
   <si>
-    <t>q41</t>
-  </si>
-  <si>
     <t>q21,q7</t>
   </si>
   <si>
@@ -369,6 +354,9 @@
   </si>
   <si>
     <t>Q48</t>
+  </si>
+  <si>
+    <t>q2,q30</t>
   </si>
 </sst>
 </file>
@@ -705,7 +693,7 @@
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+      <selection activeCell="X16" sqref="X16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,58 +759,58 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C2" t="s">
         <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s">
         <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="I2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="J2" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P2" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -830,58 +818,58 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E3" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -889,58 +877,58 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -948,58 +936,58 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -1007,58 +995,58 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1066,58 +1054,58 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1125,176 +1113,176 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>100</v>
+      <c r="B9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>79</v>
+        <v>95</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>76</v>
+      <c r="B10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1302,58 +1290,58 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="S11" s="3" t="s">
-        <v>77</v>
+        <v>95</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1361,58 +1349,58 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -1420,58 +1408,58 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1479,58 +1467,58 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1538,58 +1526,58 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1597,58 +1585,58 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q16" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="O16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="R16" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -1656,58 +1644,58 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1715,58 +1703,58 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -1774,58 +1762,58 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -1833,58 +1821,58 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N20" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -1892,58 +1880,58 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -1951,58 +1939,58 @@
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -2010,58 +1998,58 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>65</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -2069,58 +2057,58 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -2128,58 +2116,58 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -2187,58 +2175,58 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -2246,58 +2234,58 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -2332,31 +2320,31 @@
         <v>64</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -2391,31 +2379,31 @@
         <v>64</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -2423,58 +2411,58 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -2482,58 +2470,58 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -2541,58 +2529,58 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -2600,58 +2588,58 @@
         <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -2659,58 +2647,58 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -2718,58 +2706,58 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -2777,58 +2765,58 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -2836,58 +2824,58 @@
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -2895,58 +2883,58 @@
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -2954,58 +2942,58 @@
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -3013,58 +3001,58 @@
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
@@ -3072,58 +3060,58 @@
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q41" s="3" t="s">
         <v>68</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -3131,58 +3119,58 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
@@ -3190,58 +3178,58 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
@@ -3249,58 +3237,58 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
@@ -3308,58 +3296,58 @@
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
@@ -3367,58 +3355,58 @@
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
@@ -3426,58 +3414,58 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q47" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -3485,176 +3473,176 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P48" s="3" t="s">
         <v>66</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F50" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G50" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tiny fix in q0 for v input
</commit_message>
<xml_diff>
--- a/Project 1 milestone/State Tranistions_project1.xlsx
+++ b/Project 1 milestone/State Tranistions_project1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="112">
   <si>
     <t>Q0</t>
   </si>
@@ -282,6 +282,9 @@
   </si>
   <si>
     <t>q20</t>
+  </si>
+  <si>
+    <t>q23</t>
   </si>
   <si>
     <t>q48</t>
@@ -693,7 +696,7 @@
   <dimension ref="A1:S50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X16" sqref="X16"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,58 +762,58 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F2" t="s">
         <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="I2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -818,58 +821,58 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -877,58 +880,58 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H4" t="s">
         <v>69</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -936,58 +939,58 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I5" t="s">
         <v>70</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -995,58 +998,58 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J6" t="s">
         <v>71</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -1054,58 +1057,58 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L7" t="s">
         <v>72</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -1113,58 +1116,58 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R8" t="s">
         <v>73</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -1172,58 +1175,58 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>74</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -1261,28 +1264,28 @@
         <v>82</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -1290,58 +1293,58 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>76</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -1349,55 +1352,55 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S12" s="3" t="s">
         <v>77</v>
@@ -1408,58 +1411,58 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -1494,31 +1497,31 @@
         <v>78</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -1529,55 +1532,55 @@
         <v>78</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>79</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -1588,55 +1591,55 @@
         <v>78</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>80</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -1644,58 +1647,58 @@
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>81</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -1703,55 +1706,55 @@
         <v>16</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S18" s="3" t="s">
         <v>77</v>
@@ -1762,58 +1765,58 @@
         <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>83</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -1821,55 +1824,55 @@
         <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N20" s="3" t="s">
         <v>84</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S20" s="3" t="s">
         <v>77</v>
@@ -1880,58 +1883,58 @@
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L21" s="3" t="s">
         <v>85</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -1939,58 +1942,58 @@
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -1998,58 +2001,58 @@
         <v>21</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L23" s="3" t="s">
         <v>65</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -2057,55 +2060,55 @@
         <v>22</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S24" s="3" t="s">
         <v>77</v>
@@ -2116,58 +2119,58 @@
         <v>23</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -2175,58 +2178,58 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -2234,58 +2237,58 @@
         <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L27" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -2320,31 +2323,31 @@
         <v>64</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -2379,31 +2382,31 @@
         <v>64</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -2411,58 +2414,58 @@
         <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L30" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -2470,58 +2473,58 @@
         <v>29</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -2529,58 +2532,58 @@
         <v>30</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L32" s="3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -2588,58 +2591,58 @@
         <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="K33" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="L33" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -2647,58 +2650,58 @@
         <v>32</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L34" s="3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S34" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -2706,58 +2709,58 @@
         <v>33</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N35" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -2765,58 +2768,58 @@
         <v>34</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L36" s="3" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S36" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -2824,58 +2827,58 @@
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L37" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q37" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R37" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S37" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -2883,58 +2886,58 @@
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R38" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S38" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -2942,58 +2945,58 @@
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M39" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P39" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q39" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R39" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S39" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -3001,58 +3004,58 @@
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L40" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="M40" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P40" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q40" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R40" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S40" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
@@ -3060,58 +3063,58 @@
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J41" s="3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P41" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q41" s="3" t="s">
         <v>68</v>
       </c>
       <c r="R41" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -3119,58 +3122,58 @@
         <v>40</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S42" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
@@ -3178,58 +3181,58 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S43" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
@@ -3237,58 +3240,58 @@
         <v>42</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L44" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S44" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
@@ -3296,58 +3299,58 @@
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R45" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S45" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
@@ -3355,58 +3358,58 @@
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L46" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O46" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P46" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q46" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R46" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S46" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
@@ -3414,58 +3417,58 @@
         <v>45</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q47" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="R47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S47" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -3473,176 +3476,176 @@
         <v>46</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P48" s="3" t="s">
         <v>66</v>
       </c>
       <c r="Q48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S48" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S49" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F50" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="G50" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="J50" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="Q50" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="R50" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="S50" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>